<commit_message>
Todo: Implement PC zu Default-Windowsprinter
</commit_message>
<xml_diff>
--- a/output/gilles.xlsx
+++ b/output/gilles.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Bureau" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="LieuGestion" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="LienBureauLieuGestion" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="BureauUsers" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,535 +462,520 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LE-ADM-Arbeitsbereich1</t>
+          <t>AL-ZUL-CC61</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>LE-ADM-Arbeitsbereich1</t>
+          <t>AL-ZUL-CC61</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AL-ZUL-CC61</t>
+          <t>AL-ZUL-PEZ 1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>AL-ZUL-CC61</t>
+          <t>AL-ZUL-PEZ 1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 1</t>
+          <t>AL-ZUL-PEZ 2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 1</t>
+          <t>AL-ZUL-PEZ 2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 2</t>
+          <t>AL-ZUL-PEZ 3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 2</t>
+          <t>AL-ZUL-PEZ 3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 3</t>
+          <t>AL-ZUL-PEZ 4</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 3</t>
+          <t>AL-ZUL-PEZ 4</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 4</t>
+          <t>AL-ZUL-PEZ 5</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 4</t>
+          <t>AL-ZUL-PEZ 5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 5</t>
+          <t>AL-ZUL-PEZ 6</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 5</t>
+          <t>AL-ZUL-PEZ 6</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 6</t>
+          <t>AL-ZUL-PEZ 7</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 6</t>
+          <t>AL-ZUL-PEZ 7</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 7</t>
+          <t>AL-ZUL-FZZ 1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 7</t>
+          <t>AL-ZUL-FZZ 1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 1</t>
+          <t>AL-ZUL-FZZ 2</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 1</t>
+          <t>AL-ZUL-FZZ 2</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 2</t>
+          <t>AL-ZUL-FZZ 3</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 2</t>
+          <t>AL-ZUL-FZZ 3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 3</t>
+          <t>AL-ZUL-FZZ 4</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 3</t>
+          <t>AL-ZUL-FZZ 4</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 4</t>
+          <t>AL-ZUL-FZZ 5</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 4</t>
+          <t>AL-ZUL-FZZ 5</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 5</t>
+          <t>AL-ZUL-FZZ 6</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 5</t>
+          <t>AL-ZUL-FZZ 6</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 6</t>
+          <t>AL-ZUL-FZZ 7</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 6</t>
+          <t>AL-ZUL-FZZ 7</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 7</t>
+          <t>AL-ZUL-FZZSpez1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 7</t>
+          <t>AL-ZUL-FZZSpez1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez1</t>
+          <t>AL-ZUL-FZZSpez2</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez1</t>
+          <t>AL-ZUL-FZZSpez2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez2</t>
+          <t>AL-ZUL-FZZSpez3</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez2</t>
+          <t>AL-ZUL-FZZSpez3</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez3</t>
+          <t>AL-ZUL-FZZSpez4</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez3</t>
+          <t>AL-ZUL-FZZSpez4</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez4</t>
+          <t>AL-ZUL-FZZSpez5</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez4</t>
+          <t>AL-ZUL-FZZSpez5</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez5</t>
+          <t>AL-ZUL-FZZSpez6</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez5</t>
+          <t>AL-ZUL-FZZSpez6</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez6</t>
+          <t>AL-ZUL-FZZSpez7</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez6</t>
+          <t>AL-ZUL-FZZSpez7</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez7</t>
+          <t>AL-ZUL-FZZSpez8</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez7</t>
+          <t>AL-ZUL-FZZSpez8</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez8</t>
+          <t>AL-ZUL-FZZSpez9</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez8</t>
+          <t>AL-ZUL-FZZSpez9</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez9</t>
+          <t>AL-ZUL-FZZSpez10</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez9</t>
+          <t>AL-ZUL-FZZSpez10</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez10</t>
+          <t>AL-ZUL-FZZSpez11</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez10</t>
+          <t>AL-ZUL-FZZSpez11</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez11</t>
+          <t>AL-ZUL-FZZSpez12</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez11</t>
+          <t>AL-ZUL-FZZSpez12</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez12</t>
+          <t>AL-ZUL-FZZSpez13</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez12</t>
+          <t>AL-ZUL-FZZSpez13</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez13</t>
+          <t>AL-ZUL-FZZSpez14</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez13</t>
+          <t>AL-ZUL-FZZSpez14</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez14</t>
+          <t>AL-ZUL-FZZSpez15</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez14</t>
+          <t>AL-ZUL-FZZSpez15</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez15</t>
+          <t>AL-ZUL-FZZSpez16</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez15</t>
+          <t>AL-ZUL-FZZSpez16</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez16</t>
+          <t>AL-ZUL-FZZSpez17</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez16</t>
+          <t>AL-ZUL-FZZSpez17</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez17</t>
+          <t>AL-ZUL-FZZSpez18</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez17</t>
+          <t>AL-ZUL-FZZSpez18</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez18</t>
+          <t>AL-ZUL-FZZSpez19</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez18</t>
+          <t>AL-ZUL-FZZSpez19</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez19</t>
+          <t>AL-ZUL-FZZSpez20</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
-        <is>
-          <t>AL-ZUL-FZZSpez19</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>35</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>AL-ZUL-FZZSpez20</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
         <is>
           <t>AL-ZUL-FZZSpez20</t>
         </is>
@@ -1133,7 +1119,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1166,7 +1152,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LE-ADM-Arbeitsbereich1</t>
+          <t>AL-ZUL-CC61</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1176,7 +1162,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AL-ZUL-CC61</t>
+          <t>AL-ZUL-PEZ 1</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1186,7 +1172,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 1</t>
+          <t>AL-ZUL-PEZ 2</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1196,7 +1182,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 2</t>
+          <t>AL-ZUL-PEZ 3</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1206,7 +1192,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 3</t>
+          <t>AL-ZUL-PEZ 4</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1216,7 +1202,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 4</t>
+          <t>AL-ZUL-PEZ 5</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1226,7 +1212,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 5</t>
+          <t>AL-ZUL-PEZ 6</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1236,7 +1222,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 6</t>
+          <t>AL-ZUL-PEZ 7</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1246,7 +1232,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AL-ZUL-PEZ 7</t>
+          <t>AL-ZUL-FZZ 1</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1256,7 +1242,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 1</t>
+          <t>AL-ZUL-FZZ 2</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1266,7 +1252,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 2</t>
+          <t>AL-ZUL-FZZ 3</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1276,7 +1262,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 3</t>
+          <t>AL-ZUL-FZZ 4</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1286,7 +1272,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 4</t>
+          <t>AL-ZUL-FZZ 5</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1296,7 +1282,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 5</t>
+          <t>AL-ZUL-FZZ 6</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1306,7 +1292,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 6</t>
+          <t>AL-ZUL-FZZ 7</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1316,7 +1302,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZ 7</t>
+          <t>AL-ZUL-FZZSpez1</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1326,7 +1312,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez1</t>
+          <t>AL-ZUL-FZZSpez2</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1336,7 +1322,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez2</t>
+          <t>AL-ZUL-FZZSpez3</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1346,7 +1332,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez3</t>
+          <t>AL-ZUL-FZZSpez4</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1356,7 +1342,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez4</t>
+          <t>AL-ZUL-FZZSpez5</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1366,7 +1352,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez5</t>
+          <t>AL-ZUL-FZZSpez6</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1376,7 +1362,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez6</t>
+          <t>AL-ZUL-FZZSpez7</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1386,7 +1372,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez7</t>
+          <t>AL-ZUL-FZZSpez8</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1396,7 +1382,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez8</t>
+          <t>AL-ZUL-FZZSpez9</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1406,7 +1392,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez9</t>
+          <t>AL-ZUL-FZZSpez10</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1416,7 +1402,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez10</t>
+          <t>AL-ZUL-FZZSpez11</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1426,7 +1412,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez11</t>
+          <t>AL-ZUL-FZZSpez12</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1436,7 +1422,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez12</t>
+          <t>AL-ZUL-FZZSpez13</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1446,7 +1432,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez13</t>
+          <t>AL-ZUL-FZZSpez14</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1456,7 +1442,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez14</t>
+          <t>AL-ZUL-FZZSpez15</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1466,7 +1452,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez15</t>
+          <t>AL-ZUL-FZZSpez16</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1476,7 +1462,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez16</t>
+          <t>AL-ZUL-FZZSpez17</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1486,7 +1472,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez17</t>
+          <t>AL-ZUL-FZZSpez18</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1496,7 +1482,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>AL-ZUL-FZZSpez18</t>
+          <t>AL-ZUL-FZZSpez19</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1506,21 +1492,587 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>AL-ZUL-FZZSpez20</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>root.Profiles.Bureau-id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>root.Profiles.Bureau-libelle</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>users</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>LE-AAU-Arbeitsbereich 1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{'B126CHK', 'B126GRS', 'B126GUM', 'B126VOK', 'B126PAF', 'B126MA7', 'B126CHR', 'B126PAS', 'B126AMA', 'B126BC1', 'B126JAG', 'B126SIS', 'B126ISM'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AL-ZUL-CC61</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AL-ZUL-PEZ 1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AL-ZUL-PEZ 2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AL-ZUL-PEZ 3</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AL-ZUL-PEZ 4</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AL-ZUL-PEZ 5</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>AL-ZUL-PEZ 6</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AL-ZUL-PEZ 7</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZ 1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZ 2</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZ 3</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZ 4</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZ 5</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZ 6</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZ 7</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez2</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez3</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez4</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez5</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez6</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez7</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez8</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez9</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez10</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez11</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez12</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez13</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez14</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez15</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez16</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez17</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>AL-ZUL-FZZSpez18</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>AL-ZUL-FZZSpez19</t>
         </is>
       </c>
-      <c r="B37" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>AL-ZUL-FZZSpez20</t>
         </is>
       </c>
-      <c r="B38" t="n">
-        <v>1</v>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>{'B126FRC', 'B126GRG', 'B126MAS', 'B126IMD', 'B126SMP', 'B126LOG', 'B126HNA'}</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>